<commit_message>
Adicionando mapa e melhorando vizualização
Aumentando o tamanho dos mapas

Trocando o mapa de Gastos por Distrito (2019) por Gastos Per Capita por Distrito (2020)
</commit_message>
<xml_diff>
--- a/data/gastos_2019.xlsx
+++ b/data/gastos_2019.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app_tcm_ideb-main\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yajeon\Documents\GitHub\app_tcm_ideb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{847858EC-5B71-4CD5-B71D-8AD4BD337498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A668C3-8A8C-44E1-83D1-3A0D9D62B6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E1C0DA8-F5FB-44C3-83D3-2EAE57F10A25}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$D$1:$D$97</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -625,8 +626,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -642,7 +651,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -650,12 +659,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,18 +1000,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E1D519-91CF-4064-8FE4-3E7F20C36DF3}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,8 +1024,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1002,8 +1036,9 @@
       <c r="C2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1013,8 +1048,9 @@
       <c r="C3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1024,8 +1060,9 @@
       <c r="C4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1035,8 +1072,9 @@
       <c r="C5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1046,8 +1084,9 @@
       <c r="C6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1057,8 +1096,9 @@
       <c r="C7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1068,8 +1108,9 @@
       <c r="C8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1079,8 +1120,9 @@
       <c r="C9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1090,8 +1132,9 @@
       <c r="C10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1101,8 +1144,9 @@
       <c r="C11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1112,8 +1156,9 @@
       <c r="C12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1123,8 +1168,9 @@
       <c r="C13" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1134,8 +1180,9 @@
       <c r="C14" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1145,8 +1192,9 @@
       <c r="C15" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1156,8 +1204,9 @@
       <c r="C16" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1167,8 +1216,9 @@
       <c r="C17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1178,8 +1228,9 @@
       <c r="C18" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1189,8 +1240,9 @@
       <c r="C19" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1200,8 +1252,9 @@
       <c r="C20" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1211,8 +1264,9 @@
       <c r="C21" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1222,8 +1276,9 @@
       <c r="C22" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1233,8 +1288,9 @@
       <c r="C23" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1244,8 +1300,9 @@
       <c r="C24" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1255,8 +1312,9 @@
       <c r="C25" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1266,8 +1324,9 @@
       <c r="C26" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1277,8 +1336,9 @@
       <c r="C27" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1288,8 +1348,9 @@
       <c r="C28" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1299,8 +1360,9 @@
       <c r="C29" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1310,8 +1372,9 @@
       <c r="C30" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1321,8 +1384,9 @@
       <c r="C31" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1332,8 +1396,9 @@
       <c r="C32" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1343,8 +1408,9 @@
       <c r="C33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1354,8 +1420,9 @@
       <c r="C34" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1365,8 +1432,9 @@
       <c r="C35" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -1376,8 +1444,9 @@
       <c r="C36" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -1387,8 +1456,9 @@
       <c r="C37" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
@@ -1398,8 +1468,9 @@
       <c r="C38" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -1409,8 +1480,9 @@
       <c r="C39" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1420,8 +1492,9 @@
       <c r="C40" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>41</v>
       </c>
@@ -1431,8 +1504,9 @@
       <c r="C41" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>42</v>
       </c>
@@ -1442,8 +1516,9 @@
       <c r="C42" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>43</v>
       </c>
@@ -1453,8 +1528,9 @@
       <c r="C43" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>44</v>
       </c>
@@ -1464,8 +1540,9 @@
       <c r="C44" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>45</v>
       </c>
@@ -1475,8 +1552,9 @@
       <c r="C45" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>46</v>
       </c>
@@ -1486,8 +1564,9 @@
       <c r="C46" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1497,8 +1576,9 @@
       <c r="C47" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>96</v>
       </c>
@@ -1508,8 +1588,9 @@
       <c r="C48" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1519,8 +1600,9 @@
       <c r="C49" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1530,8 +1612,9 @@
       <c r="C50" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1541,8 +1624,9 @@
       <c r="C51" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1552,8 +1636,9 @@
       <c r="C52" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1563,8 +1648,9 @@
       <c r="C53" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>32</v>
       </c>
@@ -1574,8 +1660,9 @@
       <c r="C54" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1585,8 +1672,9 @@
       <c r="C55" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1596,8 +1684,9 @@
       <c r="C56" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1607,8 +1696,9 @@
       <c r="C57" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1618,8 +1708,9 @@
       <c r="C58" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1629,8 +1720,9 @@
       <c r="C59" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1640,8 +1732,9 @@
       <c r="C60" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1651,8 +1744,9 @@
       <c r="C61" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1662,8 +1756,9 @@
       <c r="C62" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1673,8 +1768,9 @@
       <c r="C63" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1684,8 +1780,9 @@
       <c r="C64" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1695,8 +1792,9 @@
       <c r="C65" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1706,8 +1804,9 @@
       <c r="C66" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1717,8 +1816,9 @@
       <c r="C67" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1728,8 +1828,9 @@
       <c r="C68" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1739,8 +1840,9 @@
       <c r="C69" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1750,8 +1852,9 @@
       <c r="C70" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1761,8 +1864,9 @@
       <c r="C71" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1772,8 +1876,9 @@
       <c r="C72" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1783,8 +1888,9 @@
       <c r="C73" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>95</v>
       </c>
@@ -1794,8 +1900,9 @@
       <c r="C74" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>72</v>
       </c>
@@ -1805,8 +1912,9 @@
       <c r="C75" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>73</v>
       </c>
@@ -1816,8 +1924,9 @@
       <c r="C76" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>74</v>
       </c>
@@ -1827,8 +1936,9 @@
       <c r="C77" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>75</v>
       </c>
@@ -1838,8 +1948,9 @@
       <c r="C78" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>76</v>
       </c>
@@ -1849,8 +1960,9 @@
       <c r="C79" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>77</v>
       </c>
@@ -1860,8 +1972,9 @@
       <c r="C80" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>78</v>
       </c>
@@ -1871,8 +1984,9 @@
       <c r="C81" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>79</v>
       </c>
@@ -1882,8 +1996,9 @@
       <c r="C82" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>80</v>
       </c>
@@ -1893,8 +2008,9 @@
       <c r="C83" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>81</v>
       </c>
@@ -1904,8 +2020,9 @@
       <c r="C84" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>82</v>
       </c>
@@ -1915,8 +2032,9 @@
       <c r="C85" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>83</v>
       </c>
@@ -1926,8 +2044,9 @@
       <c r="C86" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>84</v>
       </c>
@@ -1937,8 +2056,9 @@
       <c r="C87" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>85</v>
       </c>
@@ -1948,8 +2068,9 @@
       <c r="C88" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>86</v>
       </c>
@@ -1959,8 +2080,9 @@
       <c r="C89" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>87</v>
       </c>
@@ -1970,8 +2092,9 @@
       <c r="C90" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>88</v>
       </c>
@@ -1981,8 +2104,9 @@
       <c r="C91" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>89</v>
       </c>
@@ -1992,8 +2116,9 @@
       <c r="C92" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>90</v>
       </c>
@@ -2003,8 +2128,9 @@
       <c r="C93" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>91</v>
       </c>
@@ -2014,8 +2140,9 @@
       <c r="C94" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>92</v>
       </c>
@@ -2025,8 +2152,9 @@
       <c r="C95" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>93</v>
       </c>
@@ -2036,8 +2164,9 @@
       <c r="C96" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2047,8 +2176,10 @@
       <c r="C97" t="s">
         <v>194</v>
       </c>
+      <c r="D97" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>